<commit_message>
Atualizado a planilha de cálculos da rede neural multicamada.
</commit_message>
<xml_diff>
--- a/redes neurais - implementacoes sem frameworks/03 - calculos - rede neural multicamada.xlsx
+++ b/redes neurais - implementacoes sem frameworks/03 - calculos - rede neural multicamada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santc\workspace-github\ai-and-data-science-studies\redes neurais - implementacoes sem frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF7CE55-7773-4654-BFC0-06026B1F8C85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3D11FE-B161-4B4D-854A-F7A1625142B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20610" yWindow="14100" windowWidth="25035" windowHeight="16320" xr2:uid="{3E71A62B-BD45-4494-896A-6744D8BCD0D4}"/>
+    <workbookView xWindow="37110" yWindow="630" windowWidth="19725" windowHeight="29925" xr2:uid="{3E71A62B-BD45-4494-896A-6744D8BCD0D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
   <si>
-    <t>Sigmoid</t>
+    <t>Pesos</t>
   </si>
   <si>
-    <t>Soma</t>
+    <t>Fução ativação: Sigmoid</t>
   </si>
   <si>
-    <t>Saída</t>
+    <t>Função Soma</t>
   </si>
 </sst>
 </file>
@@ -41,7 +41,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -60,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -109,27 +109,115 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -628,6 +716,1437 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Conector de Seta Reta 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56636334-6F7C-4524-9771-4AB6D5FE5211}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="2409825" cy="561976"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector de Seta Reta 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{714D21D8-3CF9-46E7-9A6B-D6B782B85CF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="600075" y="400050"/>
+          <a:ext cx="2409825" cy="2257426"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector de Seta Reta 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC580156-2034-4901-8105-AFEE16C6C1E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600075" y="942975"/>
+          <a:ext cx="2419350" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector de Seta Reta 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{823A315A-CDD4-4705-A6BD-292F9DBBC912}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="933450"/>
+          <a:ext cx="2447925" cy="2505075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector de Seta Reta 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D049DD-1FD7-448D-AD54-296AC62D5FDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="609600" y="1733550"/>
+          <a:ext cx="2419350" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector de Seta Reta 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19BC4EA5-F32F-4CE0-BF02-D62EE06FB9D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2657475"/>
+          <a:ext cx="2438400" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector de Seta Reta 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0886D259-59DF-4412-8814-6644848DECFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5381625" y="371475"/>
+          <a:ext cx="2447925" cy="1352550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector de Seta Reta 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{494AE57C-724A-42BA-9CAE-35D27ABE8567}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5400675" y="1704975"/>
+          <a:ext cx="2419350" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector de Seta Reta 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{018AB916-03F4-40EF-A49A-B59A8CC9E408}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5391150" y="1704975"/>
+          <a:ext cx="2428875" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector de Seta Reta 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5BBBA08-9B5B-4E8A-8029-89B3BEB8D2ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="2409825" cy="561976"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Conector de Seta Reta 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EEC2A0D-EC7E-418B-A02A-E8DC7314FA3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="600075" y="400050"/>
+          <a:ext cx="2409825" cy="2257426"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Conector de Seta Reta 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78BC2F00-6190-48E0-8D75-CBA669D9F79A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600075" y="942975"/>
+          <a:ext cx="2419350" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Conector de Seta Reta 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FE7BB10-276B-41EA-8F0B-5D180E2D39F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="933450"/>
+          <a:ext cx="2447925" cy="2505075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Conector de Seta Reta 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB145A9-3E81-4D5D-AD6F-734EAA6CDFFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="609600" y="1733550"/>
+          <a:ext cx="2419350" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Conector de Seta Reta 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32AAE54A-7D50-4590-8404-8119986AEC2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2657475"/>
+          <a:ext cx="2438400" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector de Seta Reta 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B407112-1C43-4BCB-A2CD-83BB84392E96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5381625" y="371475"/>
+          <a:ext cx="2447925" cy="1352550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Conector de Seta Reta 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2329BE65-38C5-4E22-8AB5-0A9E7D77A45D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5400675" y="1704975"/>
+          <a:ext cx="2419350" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector de Seta Reta 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58C2C4C5-973B-460F-90E2-990BAEAA25BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5391150" y="1704975"/>
+          <a:ext cx="2428875" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector de Seta Reta 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03BF1159-22AC-44E4-A7EA-38002297E9BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="2409825" cy="561976"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector de Seta Reta 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC48FDC-5BD4-4A4F-AF69-0F39A6C9487D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="600075" y="400050"/>
+          <a:ext cx="2409825" cy="2257426"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Conector de Seta Reta 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C884D46C-8C7E-4FA2-B555-23102DF7DDD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600075" y="942975"/>
+          <a:ext cx="2419350" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Conector de Seta Reta 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F56EB9-FED7-41AD-A80A-10D2F3987FC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="933450"/>
+          <a:ext cx="2447925" cy="2505075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Conector de Seta Reta 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71996891-A686-4E65-B6B6-BAC51BB4726B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="609600" y="1733550"/>
+          <a:ext cx="2419350" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Conector de Seta Reta 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9526E521-07EC-4F79-B5AA-3A35AF115AA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2657475"/>
+          <a:ext cx="2438400" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Conector de Seta Reta 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A5C5736-EBCA-4BC3-95E1-919C86DA4395}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5381625" y="371475"/>
+          <a:ext cx="2447925" cy="1352550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Conector de Seta Reta 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0553B51-EEDA-4734-BDFC-B9C46E95F257}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5400675" y="1704975"/>
+          <a:ext cx="2419350" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Conector de Seta Reta 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B7A2C5-9B1E-4153-BCD2-621A76C72DCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5391150" y="1704975"/>
+          <a:ext cx="2428875" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -928,228 +2447,1440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75A1BE9-4BFA-4192-AD10-9486CA168F4E}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:L10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="7" width="9.140625" style="4"/>
-    <col min="12" max="12" width="9.140625" style="4"/>
+    <col min="6" max="6" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="4" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1">
         <v>-0.42399999999999999</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <f>(A5*E2)+(A14*E3)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <f>1/(1+EXP(-F2))</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <v>0.35799999999999998</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>0</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="J6">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
         <v>-1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="1"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1">
         <v>-0.74</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <f>(A5*E9)+(A14*E10)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <f>1/(1+EXP(-F9))</f>
         <v>0.5</v>
       </c>
-      <c r="J9">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
         <v>-0.89300000000000002</v>
       </c>
-      <c r="L9" s="6">
+      <c r="K9" s="1"/>
+      <c r="L9" s="17">
         <f>(G2*J6)+(G9*J9)+(G18*J11)</f>
         <v>-0.38100000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="17">
+        <f>1/(1+EXP(-L9))</f>
+        <v>0.40588573188433286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1">
         <v>-0.57699999999999996</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="J11">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1">
         <v>0.14799999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>0</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
         <v>-0.96099999999999997</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="3">
         <f>(A5*E18)+(A14*E19)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="3">
         <f>1/(1+EXP(-F18))</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1">
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14">
         <v>-0.46899999999999997</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="15"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
+        <v>-0.42399999999999999</v>
+      </c>
+      <c r="F22" s="3">
+        <f>(A25*E22)+(A34*E23)</f>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="G22" s="3">
+        <f>1/(1+EXP(-F22))</f>
+        <v>0.58855620438582912</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M28" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1">
+        <v>-0.74</v>
+      </c>
+      <c r="F29" s="3">
+        <f>(A25*E29)+(A34*E30)</f>
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="G29" s="3">
+        <f>1/(1+EXP(-F29))</f>
+        <v>0.35962318536779009</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1">
+        <v>-0.89300000000000002</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="17">
+        <f>(G22*J26)+(G29*J29)+(G38*J31)</f>
+        <v>-0.27419072229935881</v>
+      </c>
+      <c r="M29" s="17">
+        <f>1/(1+EXP(-L29))</f>
+        <v>0.43187856951314224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1">
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="11"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="11"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="11"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1">
+        <v>-0.96099999999999997</v>
+      </c>
+      <c r="F38" s="3">
+        <f>(A25*E38)+(A34*E39)</f>
+        <v>-0.46899999999999997</v>
+      </c>
+      <c r="G38" s="3">
+        <f>1/(1+EXP(-F38))</f>
+        <v>0.38485295749078957</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="11"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14">
+        <v>-0.46899999999999997</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="15"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M40" s="12"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K41" s="7"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="9"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1">
+        <v>-0.42399999999999999</v>
+      </c>
+      <c r="F42" s="3">
+        <f>(A45*E42)+(A54*E43)</f>
+        <v>-0.42399999999999999</v>
+      </c>
+      <c r="G42" s="3">
+        <f>1/(1+EXP(-F42))</f>
+        <v>0.39555998258063735</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="11"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="11"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="11"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="11"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="11"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="11"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M48" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1">
+        <v>-0.74</v>
+      </c>
+      <c r="F49" s="3">
+        <f>(A45*E49)+(A54*E50)</f>
+        <v>-0.74</v>
+      </c>
+      <c r="G49" s="3">
+        <f>1/(1+EXP(-F49))</f>
+        <v>0.32300414376147701</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1">
+        <v>-0.89300000000000002</v>
+      </c>
+      <c r="K49" s="1"/>
+      <c r="L49" s="17">
+        <f>(G42*J46)+(G49*J49)+(G58*J51)</f>
+        <v>-0.25421887269441767</v>
+      </c>
+      <c r="M49" s="17">
+        <f>1/(1+EXP(-L49))</f>
+        <v>0.43678536461116163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1">
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="K51" s="1"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="11"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="11"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="11"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="11"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="11"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="11"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="11"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1">
+        <v>-0.96099999999999997</v>
+      </c>
+      <c r="F58" s="3">
+        <f>(A45*E58)+(A54*E59)</f>
+        <v>-0.96099999999999997</v>
+      </c>
+      <c r="G58" s="3">
+        <f>1/(1+EXP(-F58))</f>
+        <v>0.27667802289494681</v>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="11"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14">
+        <v>-0.46899999999999997</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="15"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M60" s="12"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" s="7"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="9"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1">
+        <v>-0.42399999999999999</v>
+      </c>
+      <c r="F62" s="3">
+        <f>(A65*E62)+(A74*E63)</f>
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="G62" s="3">
+        <f>1/(1+EXP(-F62))</f>
+        <v>0.48350598689212332</v>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="11"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="11"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="11"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>1</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="11"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="K66" s="1"/>
+      <c r="L66" s="12"/>
+      <c r="M66" s="11"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="12"/>
+      <c r="M67" s="11"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M68" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1">
+        <v>-0.74</v>
+      </c>
+      <c r="F69" s="3">
+        <f>(A65*E69)+(A74*E70)</f>
+        <v>-1.3169999999999999</v>
+      </c>
+      <c r="G69" s="3">
+        <f>1/(1+EXP(-F69))</f>
+        <v>0.21131784831127748</v>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1">
+        <v>-0.89300000000000002</v>
+      </c>
+      <c r="K69" s="1"/>
+      <c r="L69" s="17">
+        <f>(G62*J66)+(G69*J69)+(G78*J71)</f>
+        <v>-0.16834783505262085</v>
+      </c>
+      <c r="M69" s="17">
+        <f>1/(1+EXP(-L69))</f>
+        <v>0.45801215918849292</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1">
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="K71" s="1"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="11"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="11"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="12"/>
+      <c r="M73" s="11"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="11"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="12"/>
+      <c r="M75" s="11"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="11"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="12"/>
+      <c r="M77" s="11"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="10"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1">
+        <v>-0.96099999999999997</v>
+      </c>
+      <c r="F78" s="3">
+        <f>(A65*E78)+(A74*E79)</f>
+        <v>-1.43</v>
+      </c>
+      <c r="G78" s="3">
+        <f>1/(1+EXP(-F78))</f>
+        <v>0.19309868423321644</v>
+      </c>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="12"/>
+      <c r="M78" s="11"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14">
+        <v>-0.46899999999999997</v>
+      </c>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="16"/>
+      <c r="M79" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="L9:L10"/>
+  <mergeCells count="40">
+    <mergeCell ref="L69:L70"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="M69:M70"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="A34:A35"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="G18:G19"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>